<commit_message>
762 notebooks and excel sheet F261
</commit_message>
<xml_diff>
--- a/FINANCE 261/Q6.xlsx
+++ b/FINANCE 261/Q6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel D'Souza\Documents\Engineering\uni-git\FINANCE 261\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3FB57B-569C-41D6-AE52-E4F13C4581DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFD06AC-4258-4813-AF4F-F599CCEDBAE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="7980" xr2:uid="{F8B69E98-173B-4A28-9D64-3A0A296D5863}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -44,18 +44,6 @@
     <t>IBM Adj. Close</t>
   </si>
   <si>
-    <t>Pt/P0</t>
-  </si>
-  <si>
-    <t>ln(Pt/P0)</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
     <t>AAPL Return (%)</t>
   </si>
   <si>
@@ -63,9 +51,6 @@
   </si>
   <si>
     <t>IBM Return (%)</t>
-  </si>
-  <si>
-    <t>Dna's</t>
   </si>
   <si>
     <t>Portfolio Returns</t>
@@ -98,7 +83,16 @@
     <t>Portfolio</t>
   </si>
   <si>
-    <t>SD vanilla</t>
+    <t>Corrs</t>
+  </si>
+  <si>
+    <t>i) A/M</t>
+  </si>
+  <si>
+    <t>ii) M/I</t>
+  </si>
+  <si>
+    <t>iii) A/I</t>
   </si>
 </sst>
 </file>
@@ -157,30 +151,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,9 +493,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C194685-4B51-4B55-ADDF-6279E59B26D3}">
   <dimension ref="A1:N690"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,42 +505,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="L1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -561,10 +554,10 @@
         <v>5.8159960000000002</v>
       </c>
       <c r="H2"/>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="10">
+      <c r="J2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7">
         <f>LN(B397/B337)</f>
         <v>0.99555411005249028</v>
       </c>
@@ -576,10 +569,6 @@
         <f>_xlfn.STDEV.S(C3:C397)</f>
         <v>12.758125824335847</v>
       </c>
-      <c r="N2">
-        <f>STDEV(C3:C397)</f>
-        <v>12.758125824335847</v>
-      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -610,10 +599,10 @@
         <f>AVERAGE(C3,E3,G3)</f>
         <v>9.1622342161268886</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="10">
+      <c r="J3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="7">
         <f>LN(D397/D337)</f>
         <v>1.1932462670961981</v>
       </c>
@@ -625,10 +614,6 @@
         <f>_xlfn.STDEV.S(E3:E397)</f>
         <v>9.8839239077160332</v>
       </c>
-      <c r="N3">
-        <f>STDEV(E3:E397)</f>
-        <v>9.8839239077160332</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -659,10 +644,10 @@
         <f t="shared" ref="H4:H67" si="3">AVERAGE(C4,E4,G4)</f>
         <v>9.454296011739153</v>
       </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="10">
+      <c r="J4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="7">
         <f>LN(F397/F337)</f>
         <v>-0.10004150250397012</v>
       </c>
@@ -674,10 +659,6 @@
         <f>_xlfn.STDEV.S(G3:G397)</f>
         <v>7.6017487974569304</v>
       </c>
-      <c r="N4">
-        <f>STDEV(G3:G397)</f>
-        <v>7.6017487974569304</v>
-      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -738,15 +719,10 @@
         <f t="shared" si="3"/>
         <v>-9.9218238873364744</v>
       </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
+      <c r="J6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -777,14 +753,13 @@
         <f t="shared" si="3"/>
         <v>7.7050250628900949</v>
       </c>
+      <c r="J7" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="K7">
         <f>AVERAGE(H3:H397)</f>
         <v>2.1861421905245466</v>
       </c>
-      <c r="L7">
-        <f>_xlfn.STDEV.S(H3:H397)</f>
-        <v>7.8266889791405641</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -815,6 +790,13 @@
         <f t="shared" si="3"/>
         <v>-3.3447005921011317</v>
       </c>
+      <c r="J8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8">
+        <f>_xlfn.STDEV.S(H3:H397)</f>
+        <v>7.8266889791405641</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -875,6 +857,10 @@
         <f t="shared" si="3"/>
         <v>15.580021465110454</v>
       </c>
+      <c r="J10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -905,6 +891,13 @@
         <f t="shared" si="3"/>
         <v>-1.31709975068659</v>
       </c>
+      <c r="J11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11">
+        <f>CORREL(C3:C397,E3:E397)</f>
+        <v>0.41222237330406458</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -935,6 +928,13 @@
         <f t="shared" si="3"/>
         <v>31.96137465424091</v>
       </c>
+      <c r="J12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12">
+        <f>CORREL(E3:E397,G3:G397)</f>
+        <v>0.42354959293674105</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -965,6 +965,13 @@
         <f t="shared" si="3"/>
         <v>13.143913771632102</v>
       </c>
+      <c r="J13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <f>CORREL(C3:C397,G3:G397)</f>
+        <v>0.33745531238096349</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -10657,27 +10664,27 @@
       </c>
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A337" s="6">
+      <c r="A337" s="4">
         <v>41671</v>
       </c>
-      <c r="B337" s="7">
+      <c r="B337" s="5">
         <v>63.708911999999998</v>
       </c>
-      <c r="C337" s="8">
+      <c r="C337" s="6">
         <f t="shared" si="20"/>
         <v>5.1218687862298884</v>
       </c>
-      <c r="D337" s="7">
+      <c r="D337" s="5">
         <v>33.826984000000003</v>
       </c>
-      <c r="E337" s="8">
+      <c r="E337" s="6">
         <f t="shared" si="21"/>
         <v>1.2421177944382134</v>
       </c>
-      <c r="F337" s="7">
+      <c r="F337" s="5">
         <v>150.90536499999999</v>
       </c>
-      <c r="G337" s="8">
+      <c r="G337" s="6">
         <f t="shared" si="22"/>
         <v>4.805309563528537</v>
       </c>
@@ -12457,27 +12464,27 @@
       </c>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A397" s="6">
+      <c r="A397" s="4">
         <v>43497</v>
       </c>
-      <c r="B397" s="7">
+      <c r="B397" s="5">
         <v>172.41055299999999</v>
       </c>
-      <c r="C397" s="8">
+      <c r="C397" s="6">
         <f t="shared" si="24"/>
         <v>4.0314768153917102</v>
       </c>
-      <c r="D397" s="7">
+      <c r="D397" s="5">
         <v>111.553589</v>
       </c>
-      <c r="E397" s="8">
+      <c r="E397" s="6">
         <f t="shared" si="25"/>
         <v>7.2776014296321634</v>
       </c>
-      <c r="F397" s="7">
+      <c r="F397" s="5">
         <v>136.539154</v>
       </c>
-      <c r="G397" s="8">
+      <c r="G397" s="6">
         <f t="shared" si="26"/>
         <v>2.76001379735209</v>
       </c>
@@ -12488,107 +12495,113 @@
     </row>
     <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398" s="1"/>
+      <c r="B398" s="1"/>
+      <c r="C398" s="1"/>
+      <c r="D398" s="1"/>
+      <c r="E398" s="1"/>
+      <c r="F398" s="1"/>
+      <c r="G398" s="1"/>
+      <c r="H398" s="1"/>
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
-        <v>11</v>
-      </c>
-      <c r="B399" s="2">
-        <f>LN(B366/B306)</f>
-        <v>0.98454424873522561</v>
-      </c>
-      <c r="D399" s="2">
-        <f>LN(D366/D306)</f>
-        <v>0.86636921705643966</v>
-      </c>
-      <c r="F399" s="2">
-        <f>LN(F366/F306)</f>
-        <v>1.3244168601271419E-2</v>
-      </c>
+      <c r="A399" s="1"/>
+      <c r="B399" s="1"/>
+      <c r="C399" s="1"/>
+      <c r="D399" s="1"/>
+      <c r="E399" s="1"/>
+      <c r="F399" s="1"/>
+      <c r="G399" s="1"/>
+      <c r="H399" s="1"/>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A400" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B400" s="2">
-        <f>B397/B337</f>
-        <v>2.7062234715293836</v>
-      </c>
-      <c r="D400" s="2">
-        <f>D397/D337</f>
-        <v>3.2977692897480897</v>
-      </c>
-      <c r="F400" s="2">
-        <f>F397/F337</f>
-        <v>0.90479986579668659</v>
-      </c>
+      <c r="A400" s="1"/>
+      <c r="B400" s="1"/>
+      <c r="C400" s="1"/>
+      <c r="D400" s="1"/>
+      <c r="E400" s="1"/>
+      <c r="F400" s="1"/>
+      <c r="G400" s="1"/>
+      <c r="H400" s="1"/>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A401" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B401" s="9">
-        <f>LN(B400)</f>
-        <v>0.99555411005249028</v>
-      </c>
-      <c r="D401" s="9">
-        <f>LN(D400)</f>
-        <v>1.1932462670961981</v>
-      </c>
-      <c r="F401" s="9">
-        <f>LN(F400)</f>
-        <v>-0.10004150250397012</v>
-      </c>
-      <c r="H401" s="9"/>
+      <c r="A401" s="1"/>
+      <c r="B401" s="1"/>
+      <c r="C401" s="1"/>
+      <c r="D401" s="1"/>
+      <c r="E401" s="1"/>
+      <c r="F401" s="1"/>
+      <c r="G401" s="1"/>
+      <c r="H401" s="1"/>
     </row>
     <row r="402" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A402" s="1"/>
+      <c r="B402" s="1"/>
+      <c r="C402" s="1"/>
+      <c r="D402" s="1"/>
+      <c r="E402" s="1"/>
+      <c r="F402" s="1"/>
+      <c r="G402" s="1"/>
+      <c r="H402" s="1"/>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A403" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C403" s="5">
-        <f>AVERAGE(C3:C397)</f>
-        <v>3.1177342049893335</v>
-      </c>
-      <c r="E403" s="5">
-        <f>AVERAGE(E3:E397)</f>
-        <v>2.3532802423675809</v>
-      </c>
-      <c r="G403" s="5">
-        <f>AVERAGE(G3:G397)</f>
-        <v>1.0874121242167261</v>
-      </c>
+      <c r="A403" s="1"/>
+      <c r="B403" s="1"/>
+      <c r="C403" s="1"/>
+      <c r="D403" s="1"/>
+      <c r="E403" s="1"/>
+      <c r="F403" s="1"/>
+      <c r="G403" s="1"/>
+      <c r="H403" s="1"/>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A404" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C404" s="5">
-        <f>_xlfn.STDEV.S(C3:C397)</f>
-        <v>12.758125824335847</v>
-      </c>
-      <c r="E404" s="5">
-        <f>_xlfn.STDEV.S(E3:E397)</f>
-        <v>9.8839239077160332</v>
-      </c>
-      <c r="G404" s="5">
-        <f>_xlfn.STDEV.S(G3:G397)</f>
-        <v>7.6017487974569304</v>
-      </c>
+      <c r="A404" s="1"/>
+      <c r="B404" s="1"/>
+      <c r="C404" s="1"/>
+      <c r="D404" s="1"/>
+      <c r="E404" s="1"/>
+      <c r="F404" s="1"/>
+      <c r="G404" s="1"/>
+      <c r="H404" s="1"/>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A405" s="1"/>
+      <c r="B405" s="1"/>
+      <c r="C405" s="1"/>
+      <c r="D405" s="1"/>
+      <c r="E405" s="1"/>
+      <c r="F405" s="1"/>
+      <c r="G405" s="1"/>
+      <c r="H405" s="1"/>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406" s="1"/>
+      <c r="B406" s="1"/>
+      <c r="C406" s="1"/>
+      <c r="D406" s="1"/>
+      <c r="E406" s="1"/>
+      <c r="F406" s="1"/>
+      <c r="G406" s="1"/>
+      <c r="H406" s="1"/>
     </row>
     <row r="407" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A407" s="1"/>
+      <c r="B407" s="1"/>
+      <c r="C407" s="1"/>
+      <c r="D407" s="1"/>
+      <c r="E407" s="1"/>
+      <c r="F407" s="1"/>
+      <c r="G407" s="1"/>
+      <c r="H407" s="1"/>
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A408" s="1"/>
+      <c r="B408" s="1"/>
+      <c r="C408" s="1"/>
+      <c r="D408" s="1"/>
+      <c r="E408" s="1"/>
+      <c r="F408" s="1"/>
+      <c r="G408" s="1"/>
+      <c r="H408" s="1"/>
     </row>
     <row r="409" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A409" s="1"/>
@@ -13437,6 +13450,10 @@
       <c r="A690" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J6:K6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>